<commit_message>
modify the code to ensure outputing to the correct folder; delete empty column from data file
</commit_message>
<xml_diff>
--- a/data/smi_2018_v4.xlsx
+++ b/data/smi_2018_v4.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigodienstmann/Dropbox/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xindiguo/Dropbox/sage/AACR_interactome/2018/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="800" windowWidth="23640" windowHeight="17540"/>
+    <workbookView xWindow="-24840" yWindow="-8620" windowWidth="23640" windowHeight="16540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$W$111</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$V$111</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -3098,7 +3098,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3418,15 +3418,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W111"/>
+  <dimension ref="A1:V111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="T103" sqref="T103"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="156" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="15" max="15" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3472,29 +3475,29 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="P1" t="s">
         <v>928</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>929</v>
+      </c>
       <c r="R1" s="1" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>930</v>
-      </c>
-      <c r="T1" s="1" t="s">
         <v>1013</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>1014</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>931</v>
+      </c>
       <c r="V1" s="1" t="s">
-        <v>931</v>
-      </c>
-      <c r="W1" s="1" t="s">
         <v>1018</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>455</v>
       </c>
@@ -3540,29 +3543,29 @@
       <c r="O2" t="s">
         <v>651</v>
       </c>
-      <c r="Q2">
+      <c r="P2">
         <v>2034</v>
       </c>
+      <c r="Q2" t="s">
+        <v>933</v>
+      </c>
       <c r="R2" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="S2" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="T2" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U2" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V2" t="s">
-        <v>935</v>
-      </c>
-      <c r="W2" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>609</v>
       </c>
@@ -3608,29 +3611,29 @@
       <c r="O3" t="s">
         <v>651</v>
       </c>
-      <c r="Q3">
+      <c r="P3">
         <v>5478</v>
       </c>
+      <c r="Q3" t="s">
+        <v>938</v>
+      </c>
       <c r="R3" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
       <c r="S3" t="s">
-        <v>934</v>
+        <v>1019</v>
       </c>
       <c r="T3" t="s">
-        <v>1019</v>
+        <v>939</v>
       </c>
       <c r="U3" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V3" t="s">
-        <v>935</v>
-      </c>
-      <c r="W3" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>875</v>
       </c>
@@ -3676,29 +3679,29 @@
       <c r="O4" t="s">
         <v>654</v>
       </c>
-      <c r="Q4">
+      <c r="P4">
         <v>186</v>
       </c>
+      <c r="Q4" t="s">
+        <v>940</v>
+      </c>
       <c r="R4" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="S4" t="s">
-        <v>941</v>
+        <v>936</v>
       </c>
       <c r="T4" t="s">
-        <v>936</v>
+        <v>939</v>
       </c>
       <c r="U4" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V4" t="s">
-        <v>935</v>
-      </c>
-      <c r="W4" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>881</v>
       </c>
@@ -3744,29 +3747,29 @@
       <c r="O5" t="s">
         <v>651</v>
       </c>
-      <c r="Q5">
+      <c r="P5">
         <v>5752</v>
       </c>
+      <c r="Q5" t="s">
+        <v>742</v>
+      </c>
       <c r="R5" t="s">
-        <v>742</v>
+        <v>934</v>
       </c>
       <c r="S5" t="s">
-        <v>934</v>
+        <v>1020</v>
       </c>
       <c r="T5" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U5" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V5" t="s">
-        <v>935</v>
-      </c>
-      <c r="W5" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1982</v>
       </c>
@@ -3812,29 +3815,29 @@
       <c r="O6" t="s">
         <v>664</v>
       </c>
-      <c r="Q6">
+      <c r="P6">
         <v>5137</v>
       </c>
+      <c r="Q6" t="s">
+        <v>942</v>
+      </c>
       <c r="R6" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="S6" t="s">
-        <v>943</v>
+        <v>1020</v>
       </c>
       <c r="T6" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U6" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V6" t="s">
-        <v>935</v>
-      </c>
-      <c r="W6" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2017</v>
       </c>
@@ -3880,29 +3883,29 @@
       <c r="O7" t="s">
         <v>829</v>
       </c>
-      <c r="Q7">
+      <c r="P7">
         <v>5555</v>
       </c>
+      <c r="Q7" t="s">
+        <v>764</v>
+      </c>
       <c r="R7" t="s">
-        <v>764</v>
+        <v>944</v>
       </c>
       <c r="S7" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="T7" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U7" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V7" t="s">
-        <v>935</v>
-      </c>
-      <c r="W7" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2082</v>
       </c>
@@ -3948,29 +3951,29 @@
       <c r="O8" t="s">
         <v>829</v>
       </c>
-      <c r="Q8">
+      <c r="P8">
         <v>3851</v>
       </c>
+      <c r="Q8" t="s">
+        <v>945</v>
+      </c>
       <c r="R8" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="S8" t="s">
-        <v>946</v>
+        <v>936</v>
       </c>
       <c r="T8" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U8" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V8" t="s">
-        <v>947</v>
-      </c>
-      <c r="W8" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2090</v>
       </c>
@@ -4016,29 +4019,29 @@
       <c r="O9" t="s">
         <v>712</v>
       </c>
-      <c r="Q9">
+      <c r="P9">
         <v>1696</v>
       </c>
+      <c r="Q9" t="s">
+        <v>948</v>
+      </c>
       <c r="R9" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="S9" t="s">
-        <v>949</v>
+        <v>1020</v>
       </c>
       <c r="T9" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U9" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V9" t="s">
-        <v>947</v>
-      </c>
-      <c r="W9" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2186</v>
       </c>
@@ -4084,29 +4087,29 @@
       <c r="O10" t="s">
         <v>829</v>
       </c>
-      <c r="Q10">
+      <c r="P10">
         <v>4935</v>
       </c>
+      <c r="Q10" t="s">
+        <v>729</v>
+      </c>
       <c r="R10" t="s">
-        <v>729</v>
+        <v>946</v>
       </c>
       <c r="S10" t="s">
-        <v>946</v>
+        <v>1019</v>
       </c>
       <c r="T10" t="s">
-        <v>1019</v>
+        <v>939</v>
       </c>
       <c r="U10" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V10" t="s">
-        <v>947</v>
-      </c>
-      <c r="W10" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2290</v>
       </c>
@@ -4152,29 +4155,29 @@
       <c r="O11" t="s">
         <v>829</v>
       </c>
-      <c r="Q11">
+      <c r="P11">
         <v>4726</v>
       </c>
+      <c r="Q11" t="s">
+        <v>742</v>
+      </c>
       <c r="R11" t="s">
-        <v>742</v>
+        <v>946</v>
       </c>
       <c r="S11" t="s">
-        <v>946</v>
+        <v>936</v>
       </c>
       <c r="T11" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U11" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V11" t="s">
-        <v>947</v>
-      </c>
-      <c r="W11" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2320</v>
       </c>
@@ -4220,29 +4223,29 @@
       <c r="O12" t="s">
         <v>829</v>
       </c>
-      <c r="Q12">
+      <c r="P12">
         <v>869</v>
       </c>
+      <c r="Q12" t="s">
+        <v>950</v>
+      </c>
       <c r="R12" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
       <c r="S12" t="s">
-        <v>946</v>
+        <v>1019</v>
       </c>
       <c r="T12" t="s">
-        <v>1019</v>
+        <v>937</v>
       </c>
       <c r="U12" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V12" t="s">
-        <v>947</v>
-      </c>
-      <c r="W12" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2325</v>
       </c>
@@ -4288,29 +4291,29 @@
       <c r="O13" t="s">
         <v>829</v>
       </c>
-      <c r="Q13">
+      <c r="P13">
         <v>1724</v>
       </c>
+      <c r="Q13" t="s">
+        <v>951</v>
+      </c>
       <c r="R13" t="s">
-        <v>951</v>
+        <v>943</v>
       </c>
       <c r="S13" t="s">
-        <v>943</v>
+        <v>1019</v>
       </c>
       <c r="T13" t="s">
-        <v>1019</v>
+        <v>937</v>
       </c>
       <c r="U13" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V13" t="s">
-        <v>947</v>
-      </c>
-      <c r="W13" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2544</v>
       </c>
@@ -4356,29 +4359,29 @@
       <c r="O14" t="s">
         <v>829</v>
       </c>
-      <c r="Q14">
+      <c r="P14">
         <v>3758</v>
       </c>
+      <c r="Q14" t="s">
+        <v>952</v>
+      </c>
       <c r="R14" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="S14" t="s">
-        <v>953</v>
+        <v>936</v>
       </c>
       <c r="T14" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U14" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V14" t="s">
-        <v>947</v>
-      </c>
-      <c r="W14" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2562</v>
       </c>
@@ -4424,29 +4427,29 @@
       <c r="O15" t="s">
         <v>712</v>
       </c>
-      <c r="Q15">
+      <c r="P15">
         <v>1701</v>
       </c>
+      <c r="Q15" t="s">
+        <v>954</v>
+      </c>
       <c r="R15" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="S15" t="s">
-        <v>955</v>
+        <v>936</v>
       </c>
       <c r="T15" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U15" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V15" t="s">
-        <v>947</v>
-      </c>
-      <c r="W15" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2629</v>
       </c>
@@ -4492,29 +4495,29 @@
       <c r="O16" t="s">
         <v>829</v>
       </c>
-      <c r="Q16">
+      <c r="P16">
         <v>3871</v>
       </c>
+      <c r="Q16" t="s">
+        <v>956</v>
+      </c>
       <c r="R16" t="s">
-        <v>956</v>
+        <v>944</v>
       </c>
       <c r="S16" t="s">
-        <v>944</v>
+        <v>1019</v>
       </c>
       <c r="T16" t="s">
-        <v>1019</v>
+        <v>939</v>
       </c>
       <c r="U16" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V16" t="s">
-        <v>935</v>
-      </c>
-      <c r="W16" t="s">
         <v>1017</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2758</v>
       </c>
@@ -4560,29 +4563,29 @@
       <c r="O17" t="s">
         <v>712</v>
       </c>
-      <c r="Q17">
+      <c r="P17">
         <v>125</v>
       </c>
+      <c r="Q17" t="s">
+        <v>957</v>
+      </c>
       <c r="R17" t="s">
-        <v>957</v>
+        <v>680</v>
       </c>
       <c r="S17" t="s">
-        <v>680</v>
+        <v>1019</v>
       </c>
       <c r="T17" t="s">
-        <v>1019</v>
+        <v>939</v>
       </c>
       <c r="U17" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V17" t="s">
-        <v>935</v>
-      </c>
-      <c r="W17" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2853</v>
       </c>
@@ -4628,29 +4631,29 @@
       <c r="O18" t="s">
         <v>654</v>
       </c>
-      <c r="Q18">
+      <c r="P18">
         <v>469</v>
       </c>
+      <c r="Q18" t="s">
+        <v>958</v>
+      </c>
       <c r="R18" t="s">
-        <v>958</v>
+        <v>941</v>
       </c>
       <c r="S18" t="s">
-        <v>941</v>
+        <v>1019</v>
       </c>
       <c r="T18" t="s">
-        <v>1019</v>
+        <v>939</v>
       </c>
       <c r="U18" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V18" t="s">
-        <v>935</v>
-      </c>
-      <c r="W18" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2858</v>
       </c>
@@ -4696,29 +4699,29 @@
       <c r="O19" t="s">
         <v>829</v>
       </c>
-      <c r="Q19">
+      <c r="P19">
         <v>5561</v>
       </c>
+      <c r="Q19" t="s">
+        <v>753</v>
+      </c>
       <c r="R19" t="s">
-        <v>753</v>
+        <v>944</v>
       </c>
       <c r="S19" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="T19" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U19" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V19" t="s">
-        <v>935</v>
-      </c>
-      <c r="W19" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2933</v>
       </c>
@@ -4764,29 +4767,29 @@
       <c r="O20" t="s">
         <v>829</v>
       </c>
-      <c r="Q20">
+      <c r="P20">
         <v>4967</v>
       </c>
+      <c r="Q20" t="s">
+        <v>959</v>
+      </c>
       <c r="R20" t="s">
-        <v>959</v>
+        <v>944</v>
       </c>
       <c r="S20" t="s">
-        <v>944</v>
+        <v>1019</v>
       </c>
       <c r="T20" t="s">
-        <v>1019</v>
+        <v>937</v>
       </c>
       <c r="U20" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V20" t="s">
-        <v>935</v>
-      </c>
-      <c r="W20" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2952</v>
       </c>
@@ -4832,29 +4835,29 @@
       <c r="O21" t="s">
         <v>697</v>
       </c>
-      <c r="Q21">
+      <c r="P21">
         <v>4084</v>
       </c>
+      <c r="Q21" t="s">
+        <v>960</v>
+      </c>
       <c r="R21" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="S21" t="s">
-        <v>961</v>
+        <v>1020</v>
       </c>
       <c r="T21" t="s">
-        <v>1020</v>
+        <v>937</v>
       </c>
       <c r="U21" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V21" t="s">
-        <v>947</v>
-      </c>
-      <c r="W21" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2992</v>
       </c>
@@ -4900,29 +4903,29 @@
       <c r="O22" t="s">
         <v>829</v>
       </c>
-      <c r="Q22">
+      <c r="P22">
         <v>2503</v>
       </c>
+      <c r="Q22" t="s">
+        <v>945</v>
+      </c>
       <c r="R22" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="S22" t="s">
+        <v>936</v>
+      </c>
+      <c r="T22" t="s">
+        <v>939</v>
+      </c>
+      <c r="U22" t="s">
+        <v>935</v>
+      </c>
+      <c r="V22" t="s">
         <v>944</v>
       </c>
-      <c r="T22" t="s">
-        <v>936</v>
-      </c>
-      <c r="U22" t="s">
-        <v>939</v>
-      </c>
-      <c r="V22" t="s">
-        <v>935</v>
-      </c>
-      <c r="W22" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3049</v>
       </c>
@@ -4968,29 +4971,29 @@
       <c r="O23" t="s">
         <v>656</v>
       </c>
-      <c r="Q23">
+      <c r="P23">
         <v>5085</v>
       </c>
+      <c r="Q23" t="s">
+        <v>827</v>
+      </c>
       <c r="R23" t="s">
-        <v>827</v>
+        <v>962</v>
       </c>
       <c r="S23" t="s">
-        <v>962</v>
+        <v>1019</v>
       </c>
       <c r="T23" t="s">
-        <v>1019</v>
+        <v>939</v>
       </c>
       <c r="U23" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V23" t="s">
-        <v>935</v>
-      </c>
-      <c r="W23" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3070</v>
       </c>
@@ -5036,29 +5039,29 @@
       <c r="O24" t="s">
         <v>705</v>
       </c>
-      <c r="Q24">
+      <c r="P24">
         <v>4704</v>
       </c>
+      <c r="Q24" t="s">
+        <v>952</v>
+      </c>
       <c r="R24" t="s">
-        <v>952</v>
+        <v>946</v>
       </c>
       <c r="S24" t="s">
-        <v>946</v>
+        <v>1020</v>
       </c>
       <c r="T24" t="s">
-        <v>1020</v>
+        <v>937</v>
       </c>
       <c r="U24" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V24" t="s">
-        <v>947</v>
-      </c>
-      <c r="W24" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3077</v>
       </c>
@@ -5104,29 +5107,29 @@
       <c r="O25" t="s">
         <v>829</v>
       </c>
-      <c r="Q25">
+      <c r="P25">
         <v>2755</v>
       </c>
+      <c r="Q25" t="s">
+        <v>960</v>
+      </c>
       <c r="R25" t="s">
-        <v>960</v>
+        <v>944</v>
       </c>
       <c r="S25" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="T25" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U25" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V25" t="s">
-        <v>935</v>
-      </c>
-      <c r="W25" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3135</v>
       </c>
@@ -5172,29 +5175,29 @@
       <c r="O26" t="s">
         <v>654</v>
       </c>
-      <c r="Q26">
+      <c r="P26">
         <v>4880</v>
       </c>
+      <c r="Q26" t="s">
+        <v>963</v>
+      </c>
       <c r="R26" t="s">
-        <v>963</v>
+        <v>941</v>
       </c>
       <c r="S26" t="s">
-        <v>941</v>
+        <v>1020</v>
       </c>
       <c r="T26" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U26" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V26" t="s">
-        <v>935</v>
-      </c>
-      <c r="W26" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3142</v>
       </c>
@@ -5240,29 +5243,29 @@
       <c r="O27" t="s">
         <v>705</v>
       </c>
-      <c r="Q27">
+      <c r="P27">
         <v>2746</v>
       </c>
+      <c r="Q27" t="s">
+        <v>960</v>
+      </c>
       <c r="R27" t="s">
-        <v>960</v>
+        <v>946</v>
       </c>
       <c r="S27" t="s">
-        <v>946</v>
+        <v>1020</v>
       </c>
       <c r="T27" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U27" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V27" t="s">
-        <v>935</v>
-      </c>
-      <c r="W27" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3150</v>
       </c>
@@ -5308,29 +5311,29 @@
       <c r="O28" t="s">
         <v>829</v>
       </c>
-      <c r="Q28">
+      <c r="P28">
         <v>4719</v>
       </c>
+      <c r="Q28" t="s">
+        <v>964</v>
+      </c>
       <c r="R28" t="s">
-        <v>964</v>
+        <v>946</v>
       </c>
       <c r="S28" t="s">
-        <v>946</v>
+        <v>1019</v>
       </c>
       <c r="T28" t="s">
-        <v>1019</v>
+        <v>937</v>
       </c>
       <c r="U28" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V28" t="s">
-        <v>935</v>
-      </c>
-      <c r="W28" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3152</v>
       </c>
@@ -5376,29 +5379,29 @@
       <c r="O29" t="s">
         <v>830</v>
       </c>
-      <c r="Q29">
+      <c r="P29">
         <v>2032</v>
       </c>
+      <c r="Q29" t="s">
+        <v>757</v>
+      </c>
       <c r="R29" t="s">
-        <v>757</v>
+        <v>965</v>
       </c>
       <c r="S29" t="s">
-        <v>965</v>
+        <v>1020</v>
       </c>
       <c r="T29" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U29" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V29" t="s">
-        <v>935</v>
-      </c>
-      <c r="W29" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3158</v>
       </c>
@@ -5444,29 +5447,29 @@
       <c r="O30" t="s">
         <v>731</v>
       </c>
-      <c r="Q30">
+      <c r="P30">
         <v>1736</v>
       </c>
+      <c r="Q30" t="s">
+        <v>757</v>
+      </c>
       <c r="R30" t="s">
-        <v>757</v>
+        <v>965</v>
       </c>
       <c r="S30" t="s">
-        <v>965</v>
+        <v>1020</v>
       </c>
       <c r="T30" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U30" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V30" t="s">
-        <v>947</v>
-      </c>
-      <c r="W30" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3197</v>
       </c>
@@ -5512,29 +5515,29 @@
       <c r="O31" t="s">
         <v>697</v>
       </c>
-      <c r="Q31">
+      <c r="P31">
         <v>5206</v>
       </c>
+      <c r="Q31" t="s">
+        <v>966</v>
+      </c>
       <c r="R31" t="s">
-        <v>966</v>
+        <v>961</v>
       </c>
       <c r="S31" t="s">
-        <v>961</v>
+        <v>1019</v>
       </c>
       <c r="T31" t="s">
-        <v>1019</v>
+        <v>939</v>
       </c>
       <c r="U31" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V31" t="s">
-        <v>935</v>
-      </c>
-      <c r="W31" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3241</v>
       </c>
@@ -5580,29 +5583,29 @@
       <c r="O32" t="s">
         <v>667</v>
       </c>
-      <c r="Q32">
+      <c r="P32">
         <v>2868</v>
       </c>
+      <c r="Q32" t="s">
+        <v>967</v>
+      </c>
       <c r="R32" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="S32" t="s">
-        <v>968</v>
+        <v>1020</v>
       </c>
       <c r="T32" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U32" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V32" t="s">
-        <v>935</v>
-      </c>
-      <c r="W32" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3285</v>
       </c>
@@ -5648,29 +5651,29 @@
       <c r="O33" t="s">
         <v>829</v>
       </c>
-      <c r="Q33">
+      <c r="P33">
         <v>3772</v>
       </c>
+      <c r="Q33" t="s">
+        <v>969</v>
+      </c>
       <c r="R33" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="S33" t="s">
-        <v>970</v>
+        <v>1020</v>
       </c>
       <c r="T33" t="s">
-        <v>1020</v>
+        <v>937</v>
       </c>
       <c r="U33" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V33" t="s">
-        <v>947</v>
-      </c>
-      <c r="W33" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3402</v>
       </c>
@@ -5716,29 +5719,29 @@
       <c r="O34" t="s">
         <v>717</v>
       </c>
-      <c r="Q34">
+      <c r="P34">
         <v>2750</v>
       </c>
+      <c r="Q34" t="s">
+        <v>971</v>
+      </c>
       <c r="R34" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
       <c r="S34" t="s">
-        <v>965</v>
+        <v>1019</v>
       </c>
       <c r="T34" t="s">
-        <v>1019</v>
+        <v>939</v>
       </c>
       <c r="U34" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V34" t="s">
-        <v>947</v>
-      </c>
-      <c r="W34" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3522</v>
       </c>
@@ -5784,29 +5787,29 @@
       <c r="O35" t="s">
         <v>829</v>
       </c>
-      <c r="Q35">
+      <c r="P35">
         <v>3760</v>
       </c>
+      <c r="Q35" t="s">
+        <v>789</v>
+      </c>
       <c r="R35" t="s">
-        <v>789</v>
+        <v>972</v>
       </c>
       <c r="S35" t="s">
-        <v>972</v>
+        <v>1020</v>
       </c>
       <c r="T35" t="s">
-        <v>1020</v>
+        <v>937</v>
       </c>
       <c r="U35" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V35" t="s">
-        <v>947</v>
-      </c>
-      <c r="W35" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3534</v>
       </c>
@@ -5852,29 +5855,29 @@
       <c r="O36" t="s">
         <v>656</v>
       </c>
-      <c r="Q36">
+      <c r="P36">
         <v>3779</v>
       </c>
+      <c r="Q36" t="s">
+        <v>960</v>
+      </c>
       <c r="R36" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="S36" t="s">
-        <v>962</v>
+        <v>1020</v>
       </c>
       <c r="T36" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U36" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V36" t="s">
-        <v>935</v>
-      </c>
-      <c r="W36" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3537</v>
       </c>
@@ -5920,29 +5923,29 @@
       <c r="O37" t="s">
         <v>654</v>
       </c>
-      <c r="Q37">
+      <c r="P37">
         <v>1679</v>
       </c>
+      <c r="Q37" t="s">
+        <v>945</v>
+      </c>
       <c r="R37" t="s">
-        <v>945</v>
+        <v>941</v>
       </c>
       <c r="S37" t="s">
-        <v>941</v>
+        <v>936</v>
       </c>
       <c r="T37" t="s">
-        <v>936</v>
+        <v>939</v>
       </c>
       <c r="U37" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V37" t="s">
-        <v>935</v>
-      </c>
-      <c r="W37" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3556</v>
       </c>
@@ -5988,29 +5991,29 @@
       <c r="O38" t="s">
         <v>829</v>
       </c>
-      <c r="Q38">
+      <c r="P38">
         <v>2915</v>
       </c>
+      <c r="Q38" t="s">
+        <v>973</v>
+      </c>
       <c r="R38" t="s">
-        <v>973</v>
+        <v>944</v>
       </c>
       <c r="S38" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="T38" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U38" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V38" t="s">
-        <v>947</v>
-      </c>
-      <c r="W38" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3699</v>
       </c>
@@ -6056,29 +6059,29 @@
       <c r="O39" t="s">
         <v>829</v>
       </c>
-      <c r="Q39">
+      <c r="P39">
         <v>5552</v>
       </c>
+      <c r="Q39" t="s">
+        <v>945</v>
+      </c>
       <c r="R39" t="s">
-        <v>945</v>
+        <v>974</v>
       </c>
       <c r="S39" t="s">
-        <v>974</v>
+        <v>936</v>
       </c>
       <c r="T39" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U39" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V39" t="s">
-        <v>935</v>
-      </c>
-      <c r="W39" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3732</v>
       </c>
@@ -6124,29 +6127,29 @@
       <c r="O40" t="s">
         <v>707</v>
       </c>
-      <c r="Q40">
+      <c r="P40">
         <v>805</v>
       </c>
+      <c r="Q40" t="s">
+        <v>967</v>
+      </c>
       <c r="R40" t="s">
-        <v>967</v>
+        <v>944</v>
       </c>
       <c r="S40" t="s">
-        <v>944</v>
+        <v>1019</v>
       </c>
       <c r="T40" t="s">
-        <v>1019</v>
+        <v>937</v>
       </c>
       <c r="U40" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V40" t="s">
-        <v>935</v>
-      </c>
-      <c r="W40" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3759</v>
       </c>
@@ -6192,29 +6195,29 @@
       <c r="O41" t="s">
         <v>829</v>
       </c>
-      <c r="Q41">
+      <c r="P41">
         <v>3852</v>
       </c>
+      <c r="Q41" t="s">
+        <v>975</v>
+      </c>
       <c r="R41" t="s">
-        <v>975</v>
+        <v>953</v>
       </c>
       <c r="S41" t="s">
-        <v>953</v>
+        <v>1020</v>
       </c>
       <c r="T41" t="s">
-        <v>1020</v>
+        <v>937</v>
       </c>
       <c r="U41" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V41" t="s">
-        <v>947</v>
-      </c>
-      <c r="W41" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3790</v>
       </c>
@@ -6260,29 +6263,29 @@
       <c r="O42" t="s">
         <v>705</v>
       </c>
-      <c r="Q42">
+      <c r="P42">
         <v>1742</v>
       </c>
+      <c r="Q42" t="s">
+        <v>967</v>
+      </c>
       <c r="R42" t="s">
-        <v>967</v>
+        <v>972</v>
       </c>
       <c r="S42" t="s">
-        <v>972</v>
+        <v>1020</v>
       </c>
       <c r="T42" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U42" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V42" t="s">
-        <v>947</v>
-      </c>
-      <c r="W42" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3846</v>
       </c>
@@ -6328,29 +6331,29 @@
       <c r="O43" t="s">
         <v>829</v>
       </c>
-      <c r="Q43">
+      <c r="P43">
         <v>1754</v>
       </c>
+      <c r="Q43" t="s">
+        <v>709</v>
+      </c>
       <c r="R43" t="s">
-        <v>709</v>
+        <v>944</v>
       </c>
       <c r="S43" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="T43" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U43" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V43" t="s">
-        <v>947</v>
-      </c>
-      <c r="W43" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>4151</v>
       </c>
@@ -6396,29 +6399,29 @@
       <c r="O44" t="s">
         <v>829</v>
       </c>
-      <c r="Q44">
+      <c r="P44">
         <v>5554</v>
       </c>
+      <c r="Q44" t="s">
+        <v>976</v>
+      </c>
       <c r="R44" t="s">
-        <v>976</v>
+        <v>946</v>
       </c>
       <c r="S44" t="s">
-        <v>946</v>
+        <v>936</v>
       </c>
       <c r="T44" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U44" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V44" t="s">
-        <v>935</v>
-      </c>
-      <c r="W44" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>4503</v>
       </c>
@@ -6464,29 +6467,29 @@
       <c r="O45" t="s">
         <v>829</v>
       </c>
-      <c r="Q45">
+      <c r="P45">
         <v>3512</v>
       </c>
+      <c r="Q45" t="s">
+        <v>764</v>
+      </c>
       <c r="R45" t="s">
-        <v>764</v>
+        <v>946</v>
       </c>
       <c r="S45" t="s">
-        <v>946</v>
+        <v>1020</v>
       </c>
       <c r="T45" t="s">
-        <v>1020</v>
+        <v>937</v>
       </c>
       <c r="U45" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V45" t="s">
-        <v>935</v>
-      </c>
-      <c r="W45" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>4521</v>
       </c>
@@ -6532,29 +6535,29 @@
       <c r="O46" t="s">
         <v>705</v>
       </c>
-      <c r="Q46">
+      <c r="P46">
         <v>4732</v>
       </c>
+      <c r="Q46" t="s">
+        <v>977</v>
+      </c>
       <c r="R46" t="s">
-        <v>977</v>
+        <v>946</v>
       </c>
       <c r="S46" t="s">
-        <v>946</v>
+        <v>1019</v>
       </c>
       <c r="T46" t="s">
-        <v>1019</v>
+        <v>939</v>
       </c>
       <c r="U46" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V46" t="s">
-        <v>935</v>
-      </c>
-      <c r="W46" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>4571</v>
       </c>
@@ -6600,29 +6603,29 @@
       <c r="O47" t="s">
         <v>829</v>
       </c>
-      <c r="Q47">
+      <c r="P47">
         <v>5557</v>
       </c>
+      <c r="Q47" t="s">
+        <v>952</v>
+      </c>
       <c r="R47" t="s">
-        <v>952</v>
+        <v>978</v>
       </c>
       <c r="S47" t="s">
-        <v>978</v>
+        <v>1020</v>
       </c>
       <c r="T47" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U47" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V47" t="s">
-        <v>935</v>
-      </c>
-      <c r="W47" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>4634</v>
       </c>
@@ -6668,29 +6671,29 @@
       <c r="O48" t="s">
         <v>829</v>
       </c>
-      <c r="Q48">
+      <c r="P48">
         <v>5860</v>
       </c>
+      <c r="Q48" t="s">
+        <v>979</v>
+      </c>
       <c r="R48" t="s">
-        <v>979</v>
+        <v>946</v>
       </c>
       <c r="S48" t="s">
-        <v>946</v>
+        <v>936</v>
       </c>
       <c r="T48" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U48" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V48" t="s">
-        <v>947</v>
-      </c>
-      <c r="W48" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>4840</v>
       </c>
@@ -6736,29 +6739,29 @@
       <c r="O49" t="s">
         <v>829</v>
       </c>
-      <c r="Q49">
+      <c r="P49">
         <v>2758</v>
       </c>
+      <c r="Q49" t="s">
+        <v>980</v>
+      </c>
       <c r="R49" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="S49" t="s">
-        <v>981</v>
+        <v>1019</v>
       </c>
       <c r="T49" t="s">
-        <v>1019</v>
+        <v>937</v>
       </c>
       <c r="U49" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V49" t="s">
-        <v>935</v>
-      </c>
-      <c r="W49" t="s">
         <v>1017</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>5025</v>
       </c>
@@ -6804,29 +6807,29 @@
       <c r="O50" t="s">
         <v>829</v>
       </c>
-      <c r="Q50">
+      <c r="P50">
         <v>4721</v>
       </c>
+      <c r="Q50" t="s">
+        <v>976</v>
+      </c>
       <c r="R50" t="s">
-        <v>976</v>
+        <v>982</v>
       </c>
       <c r="S50" t="s">
-        <v>982</v>
+        <v>1020</v>
       </c>
       <c r="T50" t="s">
-        <v>1020</v>
+        <v>937</v>
       </c>
       <c r="U50" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V50" t="s">
-        <v>947</v>
-      </c>
-      <c r="W50" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>5044</v>
       </c>
@@ -6872,29 +6875,29 @@
       <c r="O51" t="s">
         <v>667</v>
       </c>
-      <c r="Q51">
+      <c r="P51">
         <v>111</v>
       </c>
+      <c r="Q51" t="s">
+        <v>983</v>
+      </c>
       <c r="R51" t="s">
-        <v>983</v>
+        <v>968</v>
       </c>
       <c r="S51" t="s">
-        <v>968</v>
+        <v>1019</v>
       </c>
       <c r="T51" t="s">
-        <v>1019</v>
+        <v>939</v>
       </c>
       <c r="U51" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V51" t="s">
-        <v>935</v>
-      </c>
-      <c r="W51" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>5135</v>
       </c>
@@ -6940,29 +6943,29 @@
       <c r="O52" t="s">
         <v>654</v>
       </c>
-      <c r="Q52">
+      <c r="P52">
         <v>5191</v>
       </c>
+      <c r="Q52" t="s">
+        <v>983</v>
+      </c>
       <c r="R52" t="s">
-        <v>983</v>
+        <v>941</v>
       </c>
       <c r="S52" t="s">
-        <v>941</v>
+        <v>1019</v>
       </c>
       <c r="T52" t="s">
-        <v>1019</v>
+        <v>939</v>
       </c>
       <c r="U52" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V52" t="s">
-        <v>947</v>
-      </c>
-      <c r="W52" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>5151</v>
       </c>
@@ -7008,29 +7011,29 @@
       <c r="O53" t="s">
         <v>829</v>
       </c>
-      <c r="Q53">
+      <c r="P53">
         <v>4963</v>
       </c>
+      <c r="Q53" t="s">
+        <v>984</v>
+      </c>
       <c r="R53" t="s">
-        <v>984</v>
+        <v>944</v>
       </c>
       <c r="S53" t="s">
-        <v>944</v>
+        <v>1019</v>
       </c>
       <c r="T53" t="s">
-        <v>1019</v>
+        <v>939</v>
       </c>
       <c r="U53" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V53" t="s">
-        <v>947</v>
-      </c>
-      <c r="W53" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>5170</v>
       </c>
@@ -7076,29 +7079,29 @@
       <c r="O54" t="s">
         <v>829</v>
       </c>
-      <c r="Q54">
+      <c r="P54">
         <v>2920</v>
       </c>
+      <c r="Q54" t="s">
+        <v>985</v>
+      </c>
       <c r="R54" t="s">
-        <v>985</v>
+        <v>946</v>
       </c>
       <c r="S54" t="s">
-        <v>946</v>
+        <v>936</v>
       </c>
       <c r="T54" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U54" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V54" t="s">
-        <v>947</v>
-      </c>
-      <c r="W54" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>5296</v>
       </c>
@@ -7144,29 +7147,29 @@
       <c r="O55" t="s">
         <v>667</v>
       </c>
-      <c r="Q55">
+      <c r="P55">
         <v>5121</v>
       </c>
+      <c r="Q55" t="s">
+        <v>696</v>
+      </c>
       <c r="R55" t="s">
-        <v>696</v>
+        <v>968</v>
       </c>
       <c r="S55" t="s">
-        <v>968</v>
+        <v>1020</v>
       </c>
       <c r="T55" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U55" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V55" t="s">
-        <v>935</v>
-      </c>
-      <c r="W55" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>5311</v>
       </c>
@@ -7212,29 +7215,29 @@
       <c r="O56" t="s">
         <v>712</v>
       </c>
-      <c r="Q56">
+      <c r="P56">
         <v>1749</v>
       </c>
+      <c r="Q56" t="s">
+        <v>696</v>
+      </c>
       <c r="R56" t="s">
-        <v>696</v>
+        <v>680</v>
       </c>
       <c r="S56" t="s">
-        <v>680</v>
+        <v>1020</v>
       </c>
       <c r="T56" t="s">
-        <v>1020</v>
+        <v>937</v>
       </c>
       <c r="U56" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V56" t="s">
-        <v>947</v>
-      </c>
-      <c r="W56" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>5324</v>
       </c>
@@ -7280,29 +7283,29 @@
       <c r="O57" t="s">
         <v>654</v>
       </c>
-      <c r="Q57">
+      <c r="P57">
         <v>4730</v>
       </c>
+      <c r="Q57" t="s">
+        <v>984</v>
+      </c>
       <c r="R57" t="s">
-        <v>984</v>
+        <v>941</v>
       </c>
       <c r="S57" t="s">
-        <v>941</v>
+        <v>1020</v>
       </c>
       <c r="T57" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U57" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V57" t="s">
-        <v>935</v>
-      </c>
-      <c r="W57" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>5329</v>
       </c>
@@ -7348,29 +7351,29 @@
       <c r="O58" t="s">
         <v>828</v>
       </c>
-      <c r="Q58">
+      <c r="P58">
         <v>5481</v>
       </c>
+      <c r="Q58" t="s">
+        <v>986</v>
+      </c>
       <c r="R58" t="s">
-        <v>986</v>
+        <v>965</v>
       </c>
       <c r="S58" t="s">
-        <v>965</v>
+        <v>1019</v>
       </c>
       <c r="T58" t="s">
-        <v>1019</v>
+        <v>939</v>
       </c>
       <c r="U58" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V58" t="s">
-        <v>935</v>
-      </c>
-      <c r="W58" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>5335</v>
       </c>
@@ -7416,29 +7419,29 @@
       <c r="O59" t="s">
         <v>829</v>
       </c>
-      <c r="Q59">
+      <c r="P59">
         <v>3753</v>
       </c>
+      <c r="Q59" t="s">
+        <v>987</v>
+      </c>
       <c r="R59" t="s">
-        <v>987</v>
+        <v>944</v>
       </c>
       <c r="S59" t="s">
-        <v>944</v>
+        <v>1019</v>
       </c>
       <c r="T59" t="s">
-        <v>1019</v>
+        <v>937</v>
       </c>
       <c r="U59" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V59" t="s">
-        <v>935</v>
-      </c>
-      <c r="W59" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>5395</v>
       </c>
@@ -7484,29 +7487,29 @@
       <c r="O60" t="s">
         <v>829</v>
       </c>
-      <c r="Q60">
+      <c r="P60">
         <v>5006</v>
       </c>
+      <c r="Q60" t="s">
+        <v>988</v>
+      </c>
       <c r="R60" t="s">
-        <v>988</v>
+        <v>944</v>
       </c>
       <c r="S60" t="s">
-        <v>944</v>
+        <v>1019</v>
       </c>
       <c r="T60" t="s">
-        <v>1019</v>
+        <v>939</v>
       </c>
       <c r="U60" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V60" t="s">
-        <v>935</v>
-      </c>
-      <c r="W60" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>5435</v>
       </c>
@@ -7552,29 +7555,29 @@
       <c r="O61" t="s">
         <v>829</v>
       </c>
-      <c r="Q61">
+      <c r="P61">
         <v>1757</v>
       </c>
+      <c r="Q61" t="s">
+        <v>989</v>
+      </c>
       <c r="R61" t="s">
-        <v>989</v>
+        <v>946</v>
       </c>
       <c r="S61" t="s">
-        <v>946</v>
+        <v>936</v>
       </c>
       <c r="T61" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U61" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V61" t="s">
-        <v>935</v>
-      </c>
-      <c r="W61" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>5613</v>
       </c>
@@ -7620,29 +7623,29 @@
       <c r="O62" t="s">
         <v>722</v>
       </c>
-      <c r="Q62">
+      <c r="P62">
         <v>1746</v>
       </c>
+      <c r="Q62" t="s">
+        <v>990</v>
+      </c>
       <c r="R62" t="s">
-        <v>990</v>
+        <v>962</v>
       </c>
       <c r="S62" t="s">
-        <v>962</v>
+        <v>1020</v>
       </c>
       <c r="T62" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U62" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V62" t="s">
-        <v>947</v>
-      </c>
-      <c r="W62" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>5631</v>
       </c>
@@ -7688,29 +7691,29 @@
       <c r="O63" t="s">
         <v>712</v>
       </c>
-      <c r="Q63">
+      <c r="P63">
         <v>613</v>
       </c>
+      <c r="Q63" t="s">
+        <v>696</v>
+      </c>
       <c r="R63" t="s">
-        <v>696</v>
+        <v>680</v>
       </c>
       <c r="S63" t="s">
-        <v>680</v>
+        <v>1020</v>
       </c>
       <c r="T63" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U63" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V63" t="s">
-        <v>947</v>
-      </c>
-      <c r="W63" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>5676</v>
       </c>
@@ -7756,29 +7759,29 @@
       <c r="O64" t="s">
         <v>830</v>
       </c>
-      <c r="Q64">
+      <c r="P64">
         <v>5546</v>
       </c>
+      <c r="Q64" t="s">
+        <v>765</v>
+      </c>
       <c r="R64" t="s">
-        <v>765</v>
+        <v>944</v>
       </c>
       <c r="S64" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="T64" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U64" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V64" t="s">
-        <v>935</v>
-      </c>
-      <c r="W64" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>5685</v>
       </c>
@@ -7824,29 +7827,29 @@
       <c r="O65" t="s">
         <v>829</v>
       </c>
-      <c r="Q65">
+      <c r="P65">
         <v>3855</v>
       </c>
+      <c r="Q65" t="s">
+        <v>765</v>
+      </c>
       <c r="R65" t="s">
-        <v>765</v>
+        <v>944</v>
       </c>
       <c r="S65" t="s">
-        <v>944</v>
+        <v>1019</v>
       </c>
       <c r="T65" t="s">
-        <v>1019</v>
+        <v>937</v>
       </c>
       <c r="U65" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V65" t="s">
-        <v>935</v>
-      </c>
-      <c r="W65" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>5745</v>
       </c>
@@ -7892,29 +7895,29 @@
       <c r="O66" t="s">
         <v>705</v>
       </c>
-      <c r="Q66">
+      <c r="P66">
         <v>192</v>
       </c>
+      <c r="Q66" t="s">
+        <v>764</v>
+      </c>
       <c r="R66" t="s">
-        <v>764</v>
+        <v>946</v>
       </c>
       <c r="S66" t="s">
-        <v>946</v>
+        <v>936</v>
       </c>
       <c r="T66" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U66" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V66" t="s">
-        <v>935</v>
-      </c>
-      <c r="W66" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>6119</v>
       </c>
@@ -7960,29 +7963,29 @@
       <c r="O67" t="s">
         <v>829</v>
       </c>
-      <c r="Q67">
+      <c r="P67">
         <v>2754</v>
       </c>
+      <c r="Q67" t="s">
+        <v>991</v>
+      </c>
       <c r="R67" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="S67" t="s">
-        <v>992</v>
+        <v>936</v>
       </c>
       <c r="T67" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U67" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V67" t="s">
-        <v>947</v>
-      </c>
-      <c r="W67" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>6137</v>
       </c>
@@ -8028,29 +8031,29 @@
       <c r="O68" t="s">
         <v>829</v>
       </c>
-      <c r="Q68">
+      <c r="P68">
         <v>711</v>
       </c>
+      <c r="Q68" t="s">
+        <v>960</v>
+      </c>
       <c r="R68" t="s">
-        <v>960</v>
+        <v>680</v>
       </c>
       <c r="S68" t="s">
-        <v>680</v>
+        <v>936</v>
       </c>
       <c r="T68" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U68" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V68" t="s">
-        <v>947</v>
-      </c>
-      <c r="W68" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>6200</v>
       </c>
@@ -8096,29 +8099,29 @@
       <c r="O69" t="s">
         <v>829</v>
       </c>
-      <c r="Q69">
+      <c r="P69">
         <v>1944</v>
       </c>
+      <c r="Q69" t="s">
+        <v>950</v>
+      </c>
       <c r="R69" t="s">
-        <v>950</v>
+        <v>944</v>
       </c>
       <c r="S69" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="T69" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U69" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V69" t="s">
-        <v>935</v>
-      </c>
-      <c r="W69" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>6224</v>
       </c>
@@ -8164,29 +8167,29 @@
       <c r="O70" t="s">
         <v>829</v>
       </c>
-      <c r="Q70">
+      <c r="P70">
         <v>2145</v>
       </c>
+      <c r="Q70" t="s">
+        <v>993</v>
+      </c>
       <c r="R70" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="S70" t="s">
-        <v>994</v>
+        <v>1019</v>
       </c>
       <c r="T70" t="s">
-        <v>1019</v>
+        <v>937</v>
       </c>
       <c r="U70" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V70" t="s">
-        <v>935</v>
-      </c>
-      <c r="W70" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>6279</v>
       </c>
@@ -8232,29 +8235,29 @@
       <c r="O71" t="s">
         <v>688</v>
       </c>
-      <c r="Q71">
+      <c r="P71">
         <v>4191</v>
       </c>
+      <c r="Q71" t="s">
+        <v>696</v>
+      </c>
       <c r="R71" t="s">
-        <v>696</v>
+        <v>965</v>
       </c>
       <c r="S71" t="s">
-        <v>965</v>
+        <v>1020</v>
       </c>
       <c r="T71" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U71" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V71" t="s">
-        <v>935</v>
-      </c>
-      <c r="W71" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>6327</v>
       </c>
@@ -8300,29 +8303,29 @@
       <c r="O72" t="s">
         <v>654</v>
       </c>
-      <c r="Q72">
+      <c r="P72">
         <v>919</v>
       </c>
+      <c r="Q72" t="s">
+        <v>976</v>
+      </c>
       <c r="R72" t="s">
-        <v>976</v>
+        <v>941</v>
       </c>
       <c r="S72" t="s">
-        <v>941</v>
+        <v>1019</v>
       </c>
       <c r="T72" t="s">
-        <v>1019</v>
+        <v>937</v>
       </c>
       <c r="U72" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V72" t="s">
-        <v>935</v>
-      </c>
-      <c r="W72" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>6334</v>
       </c>
@@ -8368,29 +8371,29 @@
       <c r="O73" t="s">
         <v>785</v>
       </c>
-      <c r="Q73">
+      <c r="P73">
         <v>5211</v>
       </c>
+      <c r="Q73" t="s">
+        <v>989</v>
+      </c>
       <c r="R73" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="S73" t="s">
-        <v>995</v>
+        <v>1020</v>
       </c>
       <c r="T73" t="s">
-        <v>1020</v>
+        <v>937</v>
       </c>
       <c r="U73" t="s">
-        <v>937</v>
+        <v>996</v>
       </c>
       <c r="V73" t="s">
-        <v>996</v>
-      </c>
-      <c r="W73" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>6343</v>
       </c>
@@ -8436,29 +8439,29 @@
       <c r="O74" t="s">
         <v>829</v>
       </c>
-      <c r="Q74">
+      <c r="P74">
         <v>4722</v>
       </c>
+      <c r="Q74" t="s">
+        <v>990</v>
+      </c>
       <c r="R74" t="s">
-        <v>990</v>
+        <v>946</v>
       </c>
       <c r="S74" t="s">
-        <v>946</v>
+        <v>1020</v>
       </c>
       <c r="T74" t="s">
-        <v>1020</v>
+        <v>937</v>
       </c>
       <c r="U74" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V74" t="s">
-        <v>947</v>
-      </c>
-      <c r="W74" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>6433</v>
       </c>
@@ -8504,29 +8507,29 @@
       <c r="O75" t="s">
         <v>651</v>
       </c>
-      <c r="Q75">
+      <c r="P75">
         <v>5245</v>
       </c>
+      <c r="Q75" t="s">
+        <v>764</v>
+      </c>
       <c r="R75" t="s">
-        <v>764</v>
+        <v>944</v>
       </c>
       <c r="S75" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="T75" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U75" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V75" t="s">
-        <v>947</v>
-      </c>
-      <c r="W75" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>6589</v>
       </c>
@@ -8572,29 +8575,29 @@
       <c r="O76" t="s">
         <v>705</v>
       </c>
-      <c r="Q76">
+      <c r="P76">
         <v>4904</v>
       </c>
+      <c r="Q76" t="s">
+        <v>997</v>
+      </c>
       <c r="R76" t="s">
-        <v>997</v>
+        <v>946</v>
       </c>
       <c r="S76" t="s">
-        <v>946</v>
+        <v>1020</v>
       </c>
       <c r="T76" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U76" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V76" t="s">
-        <v>947</v>
-      </c>
-      <c r="W76" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>6604</v>
       </c>
@@ -8640,29 +8643,29 @@
       <c r="O77" t="s">
         <v>712</v>
       </c>
-      <c r="Q77">
+      <c r="P77">
         <v>449</v>
       </c>
+      <c r="Q77" t="s">
+        <v>998</v>
+      </c>
       <c r="R77" t="s">
-        <v>998</v>
+        <v>680</v>
       </c>
       <c r="S77" t="s">
-        <v>680</v>
+        <v>1020</v>
       </c>
       <c r="T77" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U77" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V77" t="s">
-        <v>947</v>
-      </c>
-      <c r="W77" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>6720</v>
       </c>
@@ -8708,29 +8711,29 @@
       <c r="O78" t="s">
         <v>654</v>
       </c>
-      <c r="Q78">
+      <c r="P78">
         <v>48</v>
       </c>
+      <c r="Q78" t="s">
+        <v>999</v>
+      </c>
       <c r="R78" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="S78" t="s">
-        <v>1000</v>
+        <v>1020</v>
       </c>
       <c r="T78" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U78" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V78" t="s">
-        <v>947</v>
-      </c>
-      <c r="W78" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>6738</v>
       </c>
@@ -8776,29 +8779,29 @@
       <c r="O79" t="s">
         <v>829</v>
       </c>
-      <c r="Q79">
+      <c r="P79">
         <v>3849</v>
       </c>
+      <c r="Q79" t="s">
+        <v>976</v>
+      </c>
       <c r="R79" t="s">
-        <v>976</v>
+        <v>944</v>
       </c>
       <c r="S79" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="T79" t="s">
-        <v>936</v>
+        <v>939</v>
       </c>
       <c r="U79" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V79" t="s">
-        <v>935</v>
-      </c>
-      <c r="W79" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>6912</v>
       </c>
@@ -8844,29 +8847,29 @@
       <c r="O80" t="s">
         <v>829</v>
       </c>
-      <c r="Q80">
+      <c r="P80">
         <v>3755</v>
       </c>
+      <c r="Q80" t="s">
+        <v>960</v>
+      </c>
       <c r="R80" t="s">
-        <v>960</v>
+        <v>944</v>
       </c>
       <c r="S80" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="T80" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U80" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V80" t="s">
-        <v>947</v>
-      </c>
-      <c r="W80" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>6914</v>
       </c>
@@ -8912,29 +8915,29 @@
       <c r="O81" t="s">
         <v>651</v>
       </c>
-      <c r="Q81">
+      <c r="P81">
         <v>4065</v>
       </c>
+      <c r="Q81" t="s">
+        <v>950</v>
+      </c>
       <c r="R81" t="s">
-        <v>950</v>
+        <v>934</v>
       </c>
       <c r="S81" t="s">
-        <v>934</v>
+        <v>1020</v>
       </c>
       <c r="T81" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U81" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V81" t="s">
-        <v>947</v>
-      </c>
-      <c r="W81" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>7006</v>
       </c>
@@ -8980,29 +8983,29 @@
       <c r="O82" t="s">
         <v>829</v>
       </c>
-      <c r="Q82">
+      <c r="P82">
         <v>3756</v>
       </c>
+      <c r="Q82" t="s">
+        <v>1001</v>
+      </c>
       <c r="R82" t="s">
-        <v>1001</v>
+        <v>944</v>
       </c>
       <c r="S82" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="T82" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U82" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V82" t="s">
-        <v>935</v>
-      </c>
-      <c r="W82" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>7149</v>
       </c>
@@ -9048,29 +9051,29 @@
       <c r="O83" t="s">
         <v>705</v>
       </c>
-      <c r="Q83">
+      <c r="P83">
         <v>5667</v>
       </c>
+      <c r="Q83" t="s">
+        <v>997</v>
+      </c>
       <c r="R83" t="s">
-        <v>997</v>
+        <v>946</v>
       </c>
       <c r="S83" t="s">
-        <v>946</v>
+        <v>1019</v>
       </c>
       <c r="T83" t="s">
-        <v>1019</v>
+        <v>939</v>
       </c>
       <c r="U83" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V83" t="s">
-        <v>935</v>
-      </c>
-      <c r="W83" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>7220</v>
       </c>
@@ -9116,29 +9119,29 @@
       <c r="O84" t="s">
         <v>664</v>
       </c>
-      <c r="Q84">
+      <c r="P84">
         <v>3133</v>
       </c>
+      <c r="Q84" t="s">
+        <v>1002</v>
+      </c>
       <c r="R84" t="s">
-        <v>1002</v>
+        <v>943</v>
       </c>
       <c r="S84" t="s">
-        <v>943</v>
+        <v>1020</v>
       </c>
       <c r="T84" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U84" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V84" t="s">
-        <v>935</v>
-      </c>
-      <c r="W84" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>7250</v>
       </c>
@@ -9184,29 +9187,29 @@
       <c r="O85" t="s">
         <v>664</v>
       </c>
-      <c r="Q85">
+      <c r="P85">
         <v>3877</v>
       </c>
+      <c r="Q85" t="s">
+        <v>1003</v>
+      </c>
       <c r="R85" t="s">
-        <v>1003</v>
+        <v>943</v>
       </c>
       <c r="S85" t="s">
-        <v>943</v>
+        <v>1020</v>
       </c>
       <c r="T85" t="s">
-        <v>1020</v>
+        <v>937</v>
       </c>
       <c r="U85" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V85" t="s">
-        <v>947</v>
-      </c>
-      <c r="W85" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>7410</v>
       </c>
@@ -9252,29 +9255,29 @@
       <c r="O86" t="s">
         <v>829</v>
       </c>
-      <c r="Q86">
+      <c r="P86">
         <v>3771</v>
       </c>
+      <c r="Q86" t="s">
+        <v>1004</v>
+      </c>
       <c r="R86" t="s">
-        <v>1004</v>
+        <v>944</v>
       </c>
       <c r="S86" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="T86" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U86" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V86" t="s">
-        <v>935</v>
-      </c>
-      <c r="W86" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>7423</v>
       </c>
@@ -9320,29 +9323,29 @@
       <c r="O87" t="s">
         <v>705</v>
       </c>
-      <c r="Q87">
+      <c r="P87">
         <v>1745</v>
       </c>
+      <c r="Q87" t="s">
+        <v>789</v>
+      </c>
       <c r="R87" t="s">
-        <v>789</v>
+        <v>946</v>
       </c>
       <c r="S87" t="s">
-        <v>946</v>
+        <v>1020</v>
       </c>
       <c r="T87" t="s">
-        <v>1020</v>
+        <v>937</v>
       </c>
       <c r="U87" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V87" t="s">
-        <v>947</v>
-      </c>
-      <c r="W87" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>7441</v>
       </c>
@@ -9388,29 +9391,29 @@
       <c r="O88" t="s">
         <v>829</v>
       </c>
-      <c r="Q88">
+      <c r="P88">
         <v>4752</v>
       </c>
+      <c r="Q88" t="s">
+        <v>1005</v>
+      </c>
       <c r="R88" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="S88" t="s">
-        <v>1006</v>
+        <v>1019</v>
       </c>
       <c r="T88" t="s">
-        <v>1019</v>
+        <v>937</v>
       </c>
       <c r="U88" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V88" t="s">
-        <v>947</v>
-      </c>
-      <c r="W88" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>7442</v>
       </c>
@@ -9456,29 +9459,29 @@
       <c r="O89" t="s">
         <v>829</v>
       </c>
-      <c r="Q89">
+      <c r="P89">
         <v>3757</v>
       </c>
+      <c r="Q89" t="s">
+        <v>985</v>
+      </c>
       <c r="R89" t="s">
-        <v>985</v>
+        <v>944</v>
       </c>
       <c r="S89" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="T89" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U89" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V89" t="s">
-        <v>947</v>
-      </c>
-      <c r="W89" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>7521</v>
       </c>
@@ -9524,29 +9527,29 @@
       <c r="O90" t="s">
         <v>829</v>
       </c>
-      <c r="Q90">
+      <c r="P90">
         <v>3767</v>
       </c>
+      <c r="Q90" t="s">
+        <v>1007</v>
+      </c>
       <c r="R90" t="s">
-        <v>1007</v>
+        <v>680</v>
       </c>
       <c r="S90" t="s">
-        <v>680</v>
+        <v>1019</v>
       </c>
       <c r="T90" t="s">
-        <v>1019</v>
+        <v>937</v>
       </c>
       <c r="U90" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V90" t="s">
-        <v>947</v>
-      </c>
-      <c r="W90" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>7608</v>
       </c>
@@ -9592,29 +9595,29 @@
       <c r="O91" t="s">
         <v>829</v>
       </c>
-      <c r="Q91">
+      <c r="P91">
         <v>4723</v>
       </c>
+      <c r="Q91" t="s">
+        <v>964</v>
+      </c>
       <c r="R91" t="s">
-        <v>964</v>
+        <v>982</v>
       </c>
       <c r="S91" t="s">
-        <v>982</v>
+        <v>1019</v>
       </c>
       <c r="T91" t="s">
-        <v>1019</v>
+        <v>937</v>
       </c>
       <c r="U91" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V91" t="s">
-        <v>947</v>
-      </c>
-      <c r="W91" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>7627</v>
       </c>
@@ -9660,29 +9663,29 @@
       <c r="O92" t="s">
         <v>829</v>
       </c>
-      <c r="Q92">
+      <c r="P92">
         <v>5668</v>
       </c>
+      <c r="Q92" t="s">
+        <v>945</v>
+      </c>
       <c r="R92" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="S92" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="T92" t="s">
-        <v>936</v>
+        <v>939</v>
       </c>
       <c r="U92" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V92" t="s">
-        <v>935</v>
-      </c>
-      <c r="W92" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>7868</v>
       </c>
@@ -9728,29 +9731,29 @@
       <c r="O93" t="s">
         <v>722</v>
       </c>
-      <c r="Q93">
+      <c r="P93">
         <v>4502</v>
       </c>
+      <c r="Q93" t="s">
+        <v>749</v>
+      </c>
       <c r="R93" t="s">
-        <v>749</v>
+        <v>962</v>
       </c>
       <c r="S93" t="s">
-        <v>962</v>
+        <v>1020</v>
       </c>
       <c r="T93" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U93" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V93" t="s">
-        <v>935</v>
-      </c>
-      <c r="W93" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>7958</v>
       </c>
@@ -9796,29 +9799,29 @@
       <c r="O94" t="s">
         <v>712</v>
       </c>
-      <c r="Q94">
+      <c r="P94">
         <v>4961</v>
       </c>
+      <c r="Q94" t="s">
+        <v>1008</v>
+      </c>
       <c r="R94" t="s">
-        <v>1008</v>
+        <v>680</v>
       </c>
       <c r="S94" t="s">
-        <v>680</v>
+        <v>1020</v>
       </c>
       <c r="T94" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U94" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V94" t="s">
-        <v>935</v>
-      </c>
-      <c r="W94" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>8050</v>
       </c>
@@ -9864,29 +9867,29 @@
       <c r="O95" t="s">
         <v>712</v>
       </c>
-      <c r="Q95">
+      <c r="P95">
         <v>1703</v>
       </c>
+      <c r="Q95" t="s">
+        <v>1009</v>
+      </c>
       <c r="R95" t="s">
-        <v>1009</v>
+        <v>680</v>
       </c>
       <c r="S95" t="s">
-        <v>680</v>
+        <v>1020</v>
       </c>
       <c r="T95" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U95" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V95" t="s">
-        <v>947</v>
-      </c>
-      <c r="W95" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>8151</v>
       </c>
@@ -9932,29 +9935,29 @@
       <c r="O96" t="s">
         <v>664</v>
       </c>
-      <c r="Q96">
+      <c r="P96">
         <v>1716</v>
       </c>
+      <c r="Q96" t="s">
+        <v>951</v>
+      </c>
       <c r="R96" t="s">
-        <v>951</v>
+        <v>943</v>
       </c>
       <c r="S96" t="s">
-        <v>943</v>
+        <v>1020</v>
       </c>
       <c r="T96" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U96" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V96" t="s">
-        <v>947</v>
-      </c>
-      <c r="W96" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>8167</v>
       </c>
@@ -10000,29 +10003,29 @@
       <c r="O97" t="s">
         <v>712</v>
       </c>
-      <c r="Q97">
+      <c r="P97">
         <v>1932</v>
       </c>
+      <c r="Q97" t="s">
+        <v>1010</v>
+      </c>
       <c r="R97" t="s">
-        <v>1010</v>
+        <v>944</v>
       </c>
       <c r="S97" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="T97" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U97" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="V97" t="s">
-        <v>935</v>
-      </c>
-      <c r="W97" t="s">
         <v>1016</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>8244</v>
       </c>
@@ -10068,29 +10071,29 @@
       <c r="O98" t="s">
         <v>829</v>
       </c>
-      <c r="Q98">
+      <c r="P98">
         <v>631</v>
       </c>
+      <c r="Q98" t="s">
+        <v>976</v>
+      </c>
       <c r="R98" t="s">
-        <v>976</v>
+        <v>944</v>
       </c>
       <c r="S98" t="s">
-        <v>944</v>
+        <v>1020</v>
       </c>
       <c r="T98" t="s">
-        <v>1020</v>
+        <v>937</v>
       </c>
       <c r="U98" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V98" t="s">
-        <v>947</v>
-      </c>
-      <c r="W98" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>8314</v>
       </c>
@@ -10136,29 +10139,29 @@
       <c r="O99" t="s">
         <v>829</v>
       </c>
-      <c r="Q99">
+      <c r="P99">
         <v>3809</v>
       </c>
+      <c r="Q99" t="s">
+        <v>764</v>
+      </c>
       <c r="R99" t="s">
-        <v>764</v>
+        <v>944</v>
       </c>
       <c r="S99" t="s">
-        <v>944</v>
+        <v>1019</v>
       </c>
       <c r="T99" t="s">
-        <v>1019</v>
+        <v>937</v>
       </c>
       <c r="U99" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V99" t="s">
-        <v>947</v>
-      </c>
-      <c r="W99" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>8992</v>
       </c>
@@ -10204,29 +10207,29 @@
       <c r="O100" t="s">
         <v>829</v>
       </c>
+      <c r="P100" t="s">
+        <v>831</v>
+      </c>
       <c r="Q100" t="s">
-        <v>831</v>
+        <v>764</v>
       </c>
       <c r="R100" t="s">
-        <v>764</v>
+        <v>992</v>
       </c>
       <c r="S100" t="s">
-        <v>992</v>
+        <v>1020</v>
       </c>
       <c r="T100" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U100" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V100" t="s">
-        <v>947</v>
-      </c>
-      <c r="W100" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>9276</v>
       </c>
@@ -10272,29 +10275,29 @@
       <c r="O101" t="s">
         <v>851</v>
       </c>
+      <c r="P101" t="s">
+        <v>841</v>
+      </c>
       <c r="Q101" t="s">
-        <v>841</v>
+        <v>789</v>
       </c>
       <c r="R101" t="s">
-        <v>789</v>
+        <v>1011</v>
       </c>
       <c r="S101" t="s">
-        <v>1011</v>
+        <v>1020</v>
       </c>
       <c r="T101" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U101" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V101" t="s">
-        <v>947</v>
-      </c>
-      <c r="W101" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>9307</v>
       </c>
@@ -10340,29 +10343,29 @@
       <c r="O102" t="s">
         <v>829</v>
       </c>
+      <c r="P102" t="s">
+        <v>852</v>
+      </c>
       <c r="Q102" t="s">
-        <v>852</v>
+        <v>827</v>
       </c>
       <c r="R102" t="s">
-        <v>827</v>
+        <v>944</v>
       </c>
       <c r="S102" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="T102" t="s">
-        <v>936</v>
+        <v>939</v>
       </c>
       <c r="U102" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V102" t="s">
-        <v>935</v>
-      </c>
-      <c r="W102" t="s">
         <v>1017</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>10610</v>
       </c>
@@ -10408,29 +10411,29 @@
       <c r="O103" t="s">
         <v>712</v>
       </c>
+      <c r="P103" t="s">
+        <v>861</v>
+      </c>
       <c r="Q103" t="s">
-        <v>861</v>
+        <v>952</v>
       </c>
       <c r="R103" t="s">
-        <v>952</v>
+        <v>680</v>
       </c>
       <c r="S103" t="s">
-        <v>680</v>
+        <v>1020</v>
       </c>
       <c r="T103" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U103" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V103" t="s">
-        <v>947</v>
-      </c>
-      <c r="W103" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>10663</v>
       </c>
@@ -10476,29 +10479,29 @@
       <c r="O104" t="s">
         <v>717</v>
       </c>
+      <c r="P104" t="s">
+        <v>871</v>
+      </c>
       <c r="Q104" t="s">
-        <v>871</v>
+        <v>952</v>
       </c>
       <c r="R104" t="s">
-        <v>952</v>
+        <v>965</v>
       </c>
       <c r="S104" t="s">
-        <v>965</v>
+        <v>1020</v>
       </c>
       <c r="T104" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U104" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V104" t="s">
-        <v>947</v>
-      </c>
-      <c r="W104" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>10677</v>
       </c>
@@ -10544,29 +10547,29 @@
       <c r="O105" t="s">
         <v>829</v>
       </c>
+      <c r="P105" t="s">
+        <v>880</v>
+      </c>
       <c r="Q105" t="s">
-        <v>880</v>
+        <v>764</v>
       </c>
       <c r="R105" t="s">
-        <v>764</v>
+        <v>946</v>
       </c>
       <c r="S105" t="s">
-        <v>946</v>
+        <v>936</v>
       </c>
       <c r="T105" t="s">
-        <v>936</v>
+        <v>939</v>
       </c>
       <c r="U105" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V105" t="s">
-        <v>935</v>
-      </c>
-      <c r="W105" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>10731</v>
       </c>
@@ -10612,29 +10615,29 @@
       <c r="O106" t="s">
         <v>712</v>
       </c>
+      <c r="P106" t="s">
+        <v>888</v>
+      </c>
       <c r="Q106" t="s">
-        <v>888</v>
+        <v>952</v>
       </c>
       <c r="R106" t="s">
-        <v>952</v>
+        <v>680</v>
       </c>
       <c r="S106" t="s">
-        <v>680</v>
+        <v>1020</v>
       </c>
       <c r="T106" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U106" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V106" t="s">
-        <v>947</v>
-      </c>
-      <c r="W106" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>10771</v>
       </c>
@@ -10680,29 +10683,29 @@
       <c r="O107" t="s">
         <v>829</v>
       </c>
+      <c r="P107" t="s">
+        <v>895</v>
+      </c>
       <c r="Q107" t="s">
-        <v>895</v>
+        <v>967</v>
       </c>
       <c r="R107" t="s">
-        <v>967</v>
+        <v>1011</v>
       </c>
       <c r="S107" t="s">
-        <v>1011</v>
+        <v>936</v>
       </c>
       <c r="T107" t="s">
-        <v>936</v>
+        <v>939</v>
       </c>
       <c r="U107" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V107" t="s">
-        <v>935</v>
-      </c>
-      <c r="W107" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>10805</v>
       </c>
@@ -10748,29 +10751,29 @@
       <c r="O108" t="s">
         <v>829</v>
       </c>
+      <c r="P108" t="s">
+        <v>902</v>
+      </c>
       <c r="Q108" t="s">
-        <v>902</v>
+        <v>950</v>
       </c>
       <c r="R108" t="s">
-        <v>950</v>
+        <v>992</v>
       </c>
       <c r="S108" t="s">
-        <v>992</v>
+        <v>1020</v>
       </c>
       <c r="T108" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U108" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V108" t="s">
-        <v>935</v>
-      </c>
-      <c r="W108" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>10832</v>
       </c>
@@ -10816,29 +10819,29 @@
       <c r="O109" t="s">
         <v>688</v>
       </c>
+      <c r="P109" t="s">
+        <v>909</v>
+      </c>
       <c r="Q109" t="s">
-        <v>909</v>
+        <v>964</v>
       </c>
       <c r="R109" t="s">
-        <v>964</v>
+        <v>1012</v>
       </c>
       <c r="S109" t="s">
-        <v>1012</v>
+        <v>1020</v>
       </c>
       <c r="T109" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U109" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="V109" t="s">
-        <v>935</v>
-      </c>
-      <c r="W109" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>10861</v>
       </c>
@@ -10884,29 +10887,29 @@
       <c r="O110" t="s">
         <v>829</v>
       </c>
+      <c r="P110" t="s">
+        <v>914</v>
+      </c>
       <c r="Q110" t="s">
-        <v>914</v>
+        <v>1007</v>
       </c>
       <c r="R110" t="s">
-        <v>1007</v>
+        <v>680</v>
       </c>
       <c r="S110" t="s">
-        <v>680</v>
+        <v>1020</v>
       </c>
       <c r="T110" t="s">
-        <v>1020</v>
+        <v>937</v>
       </c>
       <c r="U110" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V110" t="s">
-        <v>947</v>
-      </c>
-      <c r="W110" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>10999</v>
       </c>
@@ -10952,30 +10955,30 @@
       <c r="O111" t="s">
         <v>654</v>
       </c>
+      <c r="P111" t="s">
+        <v>921</v>
+      </c>
       <c r="Q111" t="s">
-        <v>921</v>
+        <v>976</v>
       </c>
       <c r="R111" t="s">
-        <v>976</v>
+        <v>941</v>
       </c>
       <c r="S111" t="s">
-        <v>941</v>
+        <v>1020</v>
       </c>
       <c r="T111" t="s">
-        <v>1020</v>
+        <v>939</v>
       </c>
       <c r="U111" t="s">
-        <v>939</v>
+        <v>947</v>
       </c>
       <c r="V111" t="s">
-        <v>947</v>
-      </c>
-      <c r="W111" t="s">
         <v>1015</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W111"/>
+  <autoFilter ref="A1:V111"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>